<commit_message>
Fixed an error in the Benefit Cost template
</commit_message>
<xml_diff>
--- a/output_templates/Benefit_Cost_Template.xlsx
+++ b/output_templates/Benefit_Cost_Template.xlsx
@@ -587,8 +587,8 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="170" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="169" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1048,7 +1048,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1065,7 +1065,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1229,7 +1229,7 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1247,7 +1247,7 @@
     </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1284,10 +1284,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1315,12 +1315,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1341,6 +1335,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1540,11 +1540,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="126114816"/>
-        <c:axId val="136162304"/>
+        <c:axId val="83418496"/>
+        <c:axId val="83420672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126114816"/>
+        <c:axId val="83418496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,7 +1579,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136162304"/>
+        <c:crossAx val="83420672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1587,7 +1587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136162304"/>
+        <c:axId val="83420672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1625,7 +1625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126114816"/>
+        <c:crossAx val="83418496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1704,7 +1704,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1871,11 +1870,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53532928"/>
-        <c:axId val="53535104"/>
+        <c:axId val="84551936"/>
+        <c:axId val="84582784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53532928"/>
+        <c:axId val="84551936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1897,13 +1896,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53535104"/>
+        <c:crossAx val="84582784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1911,7 +1909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53535104"/>
+        <c:axId val="84582784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53532928"/>
+        <c:crossAx val="84551936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2189,11 +2187,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="57513472"/>
-        <c:axId val="57515392"/>
+        <c:axId val="114275840"/>
+        <c:axId val="114277760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57513472"/>
+        <c:axId val="114275840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,13 +2213,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57515392"/>
+        <c:crossAx val="114277760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2229,7 +2226,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57515392"/>
+        <c:axId val="114277760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2252,14 +2249,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57513472"/>
+        <c:crossAx val="114275840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2320,7 +2316,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2427,11 +2422,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="57538048"/>
-        <c:axId val="57539968"/>
+        <c:axId val="83517440"/>
+        <c:axId val="83519360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57538048"/>
+        <c:axId val="83517440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,7 +2461,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57539968"/>
+        <c:crossAx val="83519360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2474,7 +2469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57539968"/>
+        <c:axId val="83519360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,14 +2492,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57538048"/>
+        <c:crossAx val="83517440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2551,7 +2545,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2621,11 +2614,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="57560448"/>
-        <c:axId val="57562624"/>
+        <c:axId val="83543936"/>
+        <c:axId val="83554304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57560448"/>
+        <c:axId val="83543936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2647,13 +2640,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57562624"/>
+        <c:crossAx val="83554304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2661,7 +2653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57562624"/>
+        <c:axId val="83554304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,14 +2676,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57560448"/>
+        <c:crossAx val="83543936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2756,7 +2747,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2923,11 +2913,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="74843264"/>
-        <c:axId val="74961664"/>
+        <c:axId val="84743296"/>
+        <c:axId val="84745216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74843264"/>
+        <c:axId val="84743296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2949,13 +2939,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74961664"/>
+        <c:crossAx val="84745216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2963,7 +2952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74961664"/>
+        <c:axId val="84745216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,7 +2989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74843264"/>
+        <c:crossAx val="84743296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3241,11 +3230,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108194816"/>
-        <c:axId val="118201728"/>
+        <c:axId val="84787584"/>
+        <c:axId val="84789504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108194816"/>
+        <c:axId val="84787584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3267,13 +3256,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118201728"/>
+        <c:crossAx val="84789504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3281,7 +3269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118201728"/>
+        <c:axId val="84789504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,14 +3292,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108194816"/>
+        <c:crossAx val="84787584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3372,7 +3359,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3479,11 +3465,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="161962624"/>
-        <c:axId val="161970816"/>
+        <c:axId val="85133952"/>
+        <c:axId val="85140224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="161962624"/>
+        <c:axId val="85133952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3518,7 +3504,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161970816"/>
+        <c:crossAx val="85140224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3526,7 +3512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161970816"/>
+        <c:axId val="85140224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3549,14 +3535,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161962624"/>
+        <c:crossAx val="85133952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3603,7 +3588,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3673,11 +3657,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45488768"/>
-        <c:axId val="45519616"/>
+        <c:axId val="85181184"/>
+        <c:axId val="85183104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45488768"/>
+        <c:axId val="85181184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3699,13 +3683,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45519616"/>
+        <c:crossAx val="85183104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3713,7 +3696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45519616"/>
+        <c:axId val="85183104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,14 +3719,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45488768"/>
+        <c:crossAx val="85181184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3909,11 +3891,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="140380032"/>
-        <c:axId val="147100032"/>
+        <c:axId val="84306560"/>
+        <c:axId val="84321024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="140380032"/>
+        <c:axId val="84306560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3941,7 +3923,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147100032"/>
+        <c:crossAx val="84321024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3949,7 +3931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147100032"/>
+        <c:axId val="84321024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3979,7 +3961,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140380032"/>
+        <c:crossAx val="84306560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4159,11 +4141,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147122816"/>
-        <c:axId val="147725312"/>
+        <c:axId val="84338560"/>
+        <c:axId val="84094976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147122816"/>
+        <c:axId val="84338560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,7 +4178,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147725312"/>
+        <c:crossAx val="84094976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4204,7 +4186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147725312"/>
+        <c:axId val="84094976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4241,7 +4223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147122816"/>
+        <c:crossAx val="84338560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4516,11 +4498,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146887040"/>
-        <c:axId val="146908288"/>
+        <c:axId val="84132992"/>
+        <c:axId val="84134912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146887040"/>
+        <c:axId val="84132992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4548,7 +4530,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146908288"/>
+        <c:crossAx val="84134912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4556,7 +4538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146908288"/>
+        <c:axId val="84134912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4591,7 +4573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146887040"/>
+        <c:crossAx val="84132992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4853,11 +4835,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41403136"/>
-        <c:axId val="41405056"/>
+        <c:axId val="84173184"/>
+        <c:axId val="84175104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41403136"/>
+        <c:axId val="84173184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4885,7 +4867,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41405056"/>
+        <c:crossAx val="84175104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4893,7 +4875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41405056"/>
+        <c:axId val="84175104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4930,7 +4912,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41403136"/>
+        <c:crossAx val="84173184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5173,11 +5155,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45657472"/>
-        <c:axId val="45775104"/>
+        <c:axId val="84211584"/>
+        <c:axId val="84213760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45657472"/>
+        <c:axId val="84211584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5205,7 +5187,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45775104"/>
+        <c:crossAx val="84213760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5213,7 +5195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45775104"/>
+        <c:axId val="84213760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5243,7 +5225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45657472"/>
+        <c:crossAx val="84211584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5404,7 +5386,7 @@
                   <c:v>6.1064811565760859</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0229902685546648</c:v>
+                  <c:v>-9.5892967283748423E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.2074214612996134E-2</c:v>
@@ -5434,11 +5416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45959040"/>
-        <c:axId val="45999616"/>
+        <c:axId val="84251008"/>
+        <c:axId val="84252928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45959040"/>
+        <c:axId val="84251008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5473,7 +5455,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45999616"/>
+        <c:crossAx val="84252928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5481,7 +5463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45999616"/>
+        <c:axId val="84252928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5518,7 +5500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45959040"/>
+        <c:crossAx val="84251008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5643,11 +5625,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="46152704"/>
-        <c:axId val="49910528"/>
+        <c:axId val="84412672"/>
+        <c:axId val="84423040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46152704"/>
+        <c:axId val="84412672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5675,7 +5657,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49910528"/>
+        <c:crossAx val="84423040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5683,7 +5665,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49910528"/>
+        <c:axId val="84423040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5713,7 +5695,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46152704"/>
+        <c:crossAx val="84412672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5866,11 +5848,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149272448"/>
-        <c:axId val="149279872"/>
+        <c:axId val="84456192"/>
+        <c:axId val="84458112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149272448"/>
+        <c:axId val="84456192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5905,7 +5887,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149279872"/>
+        <c:crossAx val="84458112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5913,7 +5895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149279872"/>
+        <c:axId val="84458112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5950,7 +5932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149272448"/>
+        <c:crossAx val="84456192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8590,7 +8572,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10030,7 +10012,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10190,11 +10172,11 @@
       </c>
       <c r="M6" s="24">
         <f>F25</f>
-        <v>57875365.5899093</v>
+        <v>-1379531.1866469011</v>
       </c>
       <c r="N6" s="25">
         <f>M6/SUM('Baseline Metrics'!$C$7+'Scenario Metrics'!$C$7)/2</f>
-        <v>4.0229902685546648</v>
+        <v>-9.5892967283748423E-2</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
@@ -10275,7 +10257,7 @@
       <c r="L9" s="123" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="144">
+      <c r="M9" s="142">
         <f>HeatResults!T8</f>
         <v>6936746.666666667</v>
       </c>
@@ -10871,9 +10853,9 @@
       <c r="E25" s="63">
         <v>21</v>
       </c>
-      <c r="F25" s="92">
-        <f>RawBaseline!C83</f>
-        <v>57875365.5899093</v>
+      <c r="F25" s="61">
+        <f>'Scenario Metrics'!F25-'Baseline Metrics'!F25</f>
+        <v>-1379531.1866469011</v>
       </c>
       <c r="G25" s="28"/>
       <c r="L25" s="55" t="s">
@@ -11538,7 +11520,7 @@
       <c r="S4" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="T4" s="139" t="s">
+      <c r="T4" s="137" t="s">
         <v>144</v>
       </c>
     </row>
@@ -11546,13 +11528,13 @@
       <c r="Q5" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="R5" s="140">
+      <c r="R5" s="138">
         <v>635</v>
       </c>
-      <c r="S5" s="141">
+      <c r="S5" s="139">
         <v>196</v>
       </c>
-      <c r="T5" s="135">
+      <c r="T5" s="133">
         <f>SUM(R5:S5)</f>
         <v>831</v>
       </c>
@@ -11567,13 +11549,13 @@
       <c r="Q6" s="55" t="s">
         <v>140</v>
       </c>
-      <c r="R6" s="142">
+      <c r="R6" s="140">
         <v>1588980000</v>
       </c>
-      <c r="S6" s="143">
+      <c r="S6" s="141">
         <v>492044000</v>
       </c>
-      <c r="T6" s="136">
+      <c r="T6" s="134">
         <f t="shared" ref="T6:T8" si="0">SUM(R6:S6)</f>
         <v>2081024000</v>
       </c>
@@ -11582,15 +11564,15 @@
       <c r="Q7" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="R7" s="133">
+      <c r="R7" s="131">
         <f>R5/$V$5</f>
         <v>2.1166666666666667</v>
       </c>
-      <c r="S7" s="134">
+      <c r="S7" s="132">
         <f>S5/$V$5</f>
         <v>0.65333333333333332</v>
       </c>
-      <c r="T7" s="135">
+      <c r="T7" s="133">
         <f t="shared" si="0"/>
         <v>2.77</v>
       </c>
@@ -11599,32 +11581,32 @@
       <c r="Q8" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="R8" s="137">
+      <c r="R8" s="135">
         <f>R6/$V$5</f>
         <v>5296600</v>
       </c>
-      <c r="S8" s="138">
+      <c r="S8" s="136">
         <f>S6/$V$5</f>
         <v>1640146.6666666667</v>
       </c>
-      <c r="T8" s="138">
+      <c r="T8" s="136">
         <f t="shared" si="0"/>
         <v>6936746.666666667</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q12" s="131" t="s">
+      <c r="Q12" s="143" t="s">
         <v>145</v>
       </c>
-      <c r="R12" s="132"/>
-      <c r="S12" s="132"/>
-      <c r="T12" s="132"/>
+      <c r="R12" s="144"/>
+      <c r="S12" s="144"/>
+      <c r="T12" s="144"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q13" s="132"/>
-      <c r="R13" s="132"/>
-      <c r="S13" s="132"/>
-      <c r="T13" s="132"/>
+      <c r="Q13" s="144"/>
+      <c r="R13" s="144"/>
+      <c r="S13" s="144"/>
+      <c r="T13" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updates to BC template
</commit_message>
<xml_diff>
--- a/output_templates/Benefit_Cost_Template.xlsx
+++ b/output_templates/Benefit_Cost_Template.xlsx
@@ -9,25 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19980" windowHeight="7530"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="19980" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Charts" sheetId="12" r:id="rId1"/>
     <sheet name="Baseline Metrics" sheetId="1" r:id="rId2"/>
     <sheet name="Scenario Metrics" sheetId="9" r:id="rId3"/>
-    <sheet name="Difference" sheetId="10" r:id="rId4"/>
-    <sheet name="HeatResults" sheetId="6" r:id="rId5"/>
-    <sheet name="RawBaseline" sheetId="4" r:id="rId6"/>
-    <sheet name="RawScenario" sheetId="5" r:id="rId7"/>
-    <sheet name="Baseline Charts" sheetId="7" r:id="rId8"/>
-    <sheet name="Scenario Charts" sheetId="11" r:id="rId9"/>
+    <sheet name="BaselineScenario" sheetId="13" r:id="rId4"/>
+    <sheet name="Difference" sheetId="10" r:id="rId5"/>
+    <sheet name="HeatResults" sheetId="6" r:id="rId6"/>
+    <sheet name="RawBaseline" sheetId="4" r:id="rId7"/>
+    <sheet name="RawScenario" sheetId="5" r:id="rId8"/>
+    <sheet name="Baseline Charts" sheetId="7" r:id="rId9"/>
+    <sheet name="Scenario Charts" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="160">
   <si>
     <t xml:space="preserve">Toll and Auto Operating Cost </t>
   </si>
@@ -584,12 +585,48 @@
   <si>
     <t>2014 Base</t>
   </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>CO2 ($)</t>
+  </si>
+  <si>
+    <t>CO ($)</t>
+  </si>
+  <si>
+    <t>NO ($)</t>
+  </si>
+  <si>
+    <t>PM ($)</t>
+  </si>
+  <si>
+    <t>VOC ($)</t>
+  </si>
+  <si>
+    <t>Accident Type</t>
+  </si>
+  <si>
+    <t>per capita</t>
+  </si>
+  <si>
+    <t>Annual per Capota</t>
+  </si>
+  <si>
+    <t>Accident Type (per capita)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -600,7 +637,8 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="169" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1035,7 +1073,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1344,21 +1382,47 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7436,8 +7500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7468,12 +7532,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8718,10 +8817,7 @@
         <f>D44*C44</f>
         <v>2143019.2251708694</v>
       </c>
-      <c r="G44" s="145">
-        <f>C44/$C$7</f>
-        <v>1.0339206248107231E-2</v>
-      </c>
+      <c r="G44" s="142"/>
       <c r="H44" s="79"/>
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
@@ -8744,10 +8840,7 @@
         <f>D45*C45</f>
         <v>389651.21470448625</v>
       </c>
-      <c r="G45" s="145">
-        <f t="shared" ref="G45:G48" si="7">C45/$C$7</f>
-        <v>2.7377432967548798E-4</v>
-      </c>
+      <c r="G45" s="142"/>
       <c r="H45" s="79"/>
       <c r="I45" s="28"/>
       <c r="J45" s="28"/>
@@ -8770,10 +8863,7 @@
         <f>D46*C46</f>
         <v>324342.03928942623</v>
       </c>
-      <c r="G46" s="145">
-        <f t="shared" si="7"/>
-        <v>8.8364424585765892E-6</v>
-      </c>
+      <c r="G46" s="142"/>
       <c r="H46" s="79"/>
       <c r="I46" s="28"/>
       <c r="J46" s="28"/>
@@ -8796,10 +8886,7 @@
         <f>D47*C47</f>
         <v>8124.7655454509086</v>
       </c>
-      <c r="G47" s="145">
-        <f t="shared" si="7"/>
-        <v>2.7810994632398138E-7</v>
-      </c>
+      <c r="G47" s="142"/>
       <c r="H47" s="79"/>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
@@ -8822,10 +8909,7 @@
         <f>D48*C48</f>
         <v>267396.01091999892</v>
       </c>
-      <c r="G48" s="145">
-        <f t="shared" si="7"/>
-        <v>1.0983527806905671E-5</v>
-      </c>
+      <c r="G48" s="142"/>
       <c r="H48" s="79"/>
       <c r="I48" s="28"/>
       <c r="J48" s="28"/>
@@ -8927,8 +9011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9350,7 +9434,7 @@
       <c r="L15" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="144">
+      <c r="M15" s="56">
         <f>C15/$C$7*$R$15</f>
         <v>32.989223439693355</v>
       </c>
@@ -9414,7 +9498,7 @@
         <v>58</v>
       </c>
       <c r="M16" s="65">
-        <f t="shared" ref="M15:M20" si="6">C16/$C$7*$R$15</f>
+        <f t="shared" ref="M16:M20" si="6">C16/$C$7*$R$15</f>
         <v>14.746431361459022</v>
       </c>
       <c r="N16" s="30">
@@ -10174,7 +10258,7 @@
         <v>2488136.8453654647</v>
       </c>
       <c r="G44" s="79"/>
-      <c r="H44" s="146"/>
+      <c r="H44" s="143"/>
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
       <c r="K44" s="54"/>
@@ -10197,7 +10281,7 @@
         <v>449611.00305517408</v>
       </c>
       <c r="G45" s="79"/>
-      <c r="H45" s="146"/>
+      <c r="H45" s="143"/>
       <c r="I45" s="28"/>
       <c r="J45" s="28"/>
       <c r="K45" s="54"/>
@@ -10220,7 +10304,7 @@
         <v>372310.57044781127</v>
       </c>
       <c r="G46" s="79"/>
-      <c r="H46" s="146"/>
+      <c r="H46" s="143"/>
       <c r="I46" s="28"/>
       <c r="J46" s="28"/>
       <c r="K46" s="54"/>
@@ -10243,7 +10327,7 @@
         <v>9196.2629502295549</v>
       </c>
       <c r="G47" s="79"/>
-      <c r="H47" s="146"/>
+      <c r="H47" s="143"/>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
       <c r="K47" s="54"/>
@@ -10266,7 +10350,7 @@
         <v>314235.7630379136</v>
       </c>
       <c r="G48" s="79"/>
-      <c r="H48" s="146"/>
+      <c r="H48" s="143"/>
       <c r="I48" s="28"/>
       <c r="J48" s="28"/>
       <c r="K48" s="54"/>
@@ -10365,10 +10449,539 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="148" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="149" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="157" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="149" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="149" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" s="159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="150">
+        <f>'Baseline Metrics'!C44</f>
+        <v>38724.59749134205</v>
+      </c>
+      <c r="C3" s="144">
+        <f>'Scenario Metrics'!C44</f>
+        <v>44960.911553405575</v>
+      </c>
+      <c r="D3" s="146">
+        <f>B3-C3</f>
+        <v>-6236.314062063524</v>
+      </c>
+      <c r="F3" s="157" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="160">
+        <f>B3/'Baseline Metrics'!$C$7*300</f>
+        <v>3.1017618744321691</v>
+      </c>
+      <c r="H3" s="160">
+        <f>C3/'Scenario Metrics'!$C$7*300</f>
+        <v>2.8268087585748614</v>
+      </c>
+      <c r="I3" s="161">
+        <f>H3-G3</f>
+        <v>-0.27495311585730775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="151">
+        <f>'Baseline Metrics'!C45</f>
+        <v>1025.3979334328585</v>
+      </c>
+      <c r="C4" s="144">
+        <f>'Scenario Metrics'!C45</f>
+        <v>1183.186850145195</v>
+      </c>
+      <c r="D4" s="146">
+        <f t="shared" ref="D4:D7" si="0">B4-C4</f>
+        <v>-157.78891671233646</v>
+      </c>
+      <c r="F4" s="157" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="160">
+        <f>B4/'Baseline Metrics'!$C$7*300</f>
+        <v>8.2132298902646395E-2</v>
+      </c>
+      <c r="H4" s="160">
+        <f>C4/'Scenario Metrics'!$C$7*300</f>
+        <v>7.4390016471267431E-2</v>
+      </c>
+      <c r="I4" s="161">
+        <f t="shared" ref="I4:I7" si="1">G4-H4</f>
+        <v>7.7422824313789634E-3</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="151">
+        <f>'Baseline Metrics'!C46</f>
+        <v>33.09612645810472</v>
+      </c>
+      <c r="C5" s="144">
+        <f>'Scenario Metrics'!C46</f>
+        <v>37.990874535490946</v>
+      </c>
+      <c r="D5" s="146">
+        <f t="shared" si="0"/>
+        <v>-4.8947480773862253</v>
+      </c>
+      <c r="F5" s="157" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="160">
+        <f>B5/'Baseline Metrics'!$C$7*300</f>
+        <v>2.6509327375729766E-3</v>
+      </c>
+      <c r="H5" s="160">
+        <f>C5/'Scenario Metrics'!$C$7*300</f>
+        <v>2.3885845097975991E-3</v>
+      </c>
+      <c r="I5" s="161">
+        <f t="shared" si="1"/>
+        <v>2.6234822777537747E-4</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="151">
+        <f>'Baseline Metrics'!C47</f>
+        <v>1.0416366083911421</v>
+      </c>
+      <c r="C6" s="144">
+        <f>'Scenario Metrics'!C47</f>
+        <v>1.1790080705422505</v>
+      </c>
+      <c r="D6" s="146">
+        <f t="shared" si="0"/>
+        <v>-0.1373714621511084</v>
+      </c>
+      <c r="F6" s="157" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="160">
+        <f>B6/'Baseline Metrics'!$C$7*300</f>
+        <v>8.3432983897194414E-5</v>
+      </c>
+      <c r="H6" s="160">
+        <f>C6/'Scenario Metrics'!$C$7*300</f>
+        <v>7.4127285793137708E-5</v>
+      </c>
+      <c r="I6" s="161">
+        <f t="shared" si="1"/>
+        <v>9.3056981040567059E-6</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="152">
+        <f>'Baseline Metrics'!C48</f>
+        <v>41.137847833845989</v>
+      </c>
+      <c r="C7" s="145">
+        <f>'Scenario Metrics'!C48</f>
+        <v>48.343963544294397</v>
+      </c>
+      <c r="D7" s="147">
+        <f t="shared" si="0"/>
+        <v>-7.2061157104484082</v>
+      </c>
+      <c r="F7" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="160">
+        <f>B7/'Baseline Metrics'!$C$7*300</f>
+        <v>3.2950583420717013E-3</v>
+      </c>
+      <c r="H7" s="160">
+        <f>C7/'Scenario Metrics'!$C$7*300</f>
+        <v>3.0395099843317994E-3</v>
+      </c>
+      <c r="I7" s="161">
+        <f t="shared" si="1"/>
+        <v>2.5554835773990191E-4</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="148" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="149" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="148" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="149" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="153">
+        <f>'Baseline Metrics'!E44</f>
+        <v>2143019.2251708694</v>
+      </c>
+      <c r="C11" s="154">
+        <f>'Scenario Metrics'!E44</f>
+        <v>2488136.8453654647</v>
+      </c>
+      <c r="D11" s="146">
+        <f>B11-C11</f>
+        <v>-345117.62019459531</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="153">
+        <f>ROUND(B11,-3)</f>
+        <v>2143000</v>
+      </c>
+      <c r="H11" s="153">
+        <f t="shared" ref="H11:H15" si="2">ROUND(C11,-3)</f>
+        <v>2488000</v>
+      </c>
+      <c r="I11" s="153">
+        <f t="shared" ref="I11:I15" si="3">ROUND(D11,-3)</f>
+        <v>-345000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="153">
+        <f>'Baseline Metrics'!E45</f>
+        <v>389651.21470448625</v>
+      </c>
+      <c r="C12" s="154">
+        <f>'Scenario Metrics'!E45</f>
+        <v>449611.00305517408</v>
+      </c>
+      <c r="D12" s="146">
+        <f t="shared" ref="D12:D15" si="4">B12-C12</f>
+        <v>-59959.788350687828</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" s="153">
+        <f t="shared" ref="G12:G15" si="5">ROUND(B12,-3)</f>
+        <v>390000</v>
+      </c>
+      <c r="H12" s="153">
+        <f t="shared" si="2"/>
+        <v>450000</v>
+      </c>
+      <c r="I12" s="153">
+        <f t="shared" si="3"/>
+        <v>-60000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="153">
+        <f>'Baseline Metrics'!E46</f>
+        <v>324342.03928942623</v>
+      </c>
+      <c r="C13" s="154">
+        <f>'Scenario Metrics'!E46</f>
+        <v>372310.57044781127</v>
+      </c>
+      <c r="D13" s="146">
+        <f t="shared" si="4"/>
+        <v>-47968.531158385042</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="153">
+        <f t="shared" si="5"/>
+        <v>324000</v>
+      </c>
+      <c r="H13" s="153">
+        <f t="shared" si="2"/>
+        <v>372000</v>
+      </c>
+      <c r="I13" s="153">
+        <f t="shared" si="3"/>
+        <v>-48000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="153">
+        <f>'Baseline Metrics'!E47</f>
+        <v>8124.7655454509086</v>
+      </c>
+      <c r="C14" s="154">
+        <f>'Scenario Metrics'!E47</f>
+        <v>9196.2629502295549</v>
+      </c>
+      <c r="D14" s="146">
+        <f t="shared" si="4"/>
+        <v>-1071.4974047786463</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="153">
+        <f t="shared" si="5"/>
+        <v>8000</v>
+      </c>
+      <c r="H14" s="153">
+        <f t="shared" si="2"/>
+        <v>9000</v>
+      </c>
+      <c r="I14" s="153">
+        <f t="shared" si="3"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="153">
+        <f>'Baseline Metrics'!E48</f>
+        <v>267396.01091999892</v>
+      </c>
+      <c r="C15" s="154">
+        <f>'Scenario Metrics'!E48</f>
+        <v>314235.7630379136</v>
+      </c>
+      <c r="D15" s="147">
+        <f t="shared" si="4"/>
+        <v>-46839.752117914672</v>
+      </c>
+      <c r="F15" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="153">
+        <f t="shared" si="5"/>
+        <v>267000</v>
+      </c>
+      <c r="H15" s="153">
+        <f t="shared" si="2"/>
+        <v>314000</v>
+      </c>
+      <c r="I15" s="153">
+        <f t="shared" si="3"/>
+        <v>-47000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="A18" s="157" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="158" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="149" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="157" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="158" t="s">
+        <v>149</v>
+      </c>
+      <c r="I18" s="149" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="150">
+        <f>'Baseline Metrics'!C38</f>
+        <v>49.283153831235246</v>
+      </c>
+      <c r="C19" s="144">
+        <f>'Scenario Metrics'!C38</f>
+        <v>56.844887153160776</v>
+      </c>
+      <c r="D19" s="146">
+        <f>B19-C19</f>
+        <v>-7.56173332192553</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="150">
+        <f>B19/'Baseline Metrics'!$C$7</f>
+        <v>1.3158269550310005E-5</v>
+      </c>
+      <c r="H19" s="150" t="e">
+        <f>C19/'Baseline Metrics'!D7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="146" t="e">
+        <f>G19-H19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="A20" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="151">
+        <f>'Baseline Metrics'!C39</f>
+        <v>93.791638359199609</v>
+      </c>
+      <c r="C20" s="144">
+        <f>'Scenario Metrics'!C39</f>
+        <v>107.73371713545689</v>
+      </c>
+      <c r="D20" s="146">
+        <f t="shared" ref="D20:D21" si="6">B20-C20</f>
+        <v>-13.942078776257276</v>
+      </c>
+      <c r="F20" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="150">
+        <f>B20/'Baseline Metrics'!$C$7</f>
+        <v>2.5041734612230909E-5</v>
+      </c>
+      <c r="H20" s="150" t="e">
+        <f>C20/'Baseline Metrics'!D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="146" t="e">
+        <f t="shared" ref="I20:I21" si="7">G20-H20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="152">
+        <f>'Baseline Metrics'!C40</f>
+        <v>0.9118180229104933</v>
+      </c>
+      <c r="C21" s="145">
+        <f>'Scenario Metrics'!C40</f>
+        <v>1.0518270586399558</v>
+      </c>
+      <c r="D21" s="147">
+        <f t="shared" si="6"/>
+        <v>-0.14000903572946255</v>
+      </c>
+      <c r="F21" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="150">
+        <f>B21/'Baseline Metrics'!$C$7</f>
+        <v>2.4344925991085448E-7</v>
+      </c>
+      <c r="H21" s="150" t="e">
+        <f>C21/'Baseline Metrics'!D9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="147" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10626,7 +11239,10 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="33"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="162">
+        <f>C4*'Scenario Metrics'!C7</f>
+        <v>6766789.5369814029</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="26"/>
       <c r="F10" s="14"/>
@@ -11826,7 +12442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
@@ -11951,18 +12567,18 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q12" s="142" t="s">
+      <c r="Q12" s="155" t="s">
         <v>140</v>
       </c>
-      <c r="R12" s="143"/>
-      <c r="S12" s="143"/>
-      <c r="T12" s="143"/>
+      <c r="R12" s="156"/>
+      <c r="S12" s="156"/>
+      <c r="T12" s="156"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q13" s="143"/>
-      <c r="R13" s="143"/>
-      <c r="S13" s="143"/>
-      <c r="T13" s="143"/>
+      <c r="Q13" s="156"/>
+      <c r="R13" s="156"/>
+      <c r="S13" s="156"/>
+      <c r="T13" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11973,12 +12589,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L166"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12800,7 +13416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L166"/>
   <sheetViews>
@@ -13626,12 +14242,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13660,39 +14276,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding truck benefits calculation
</commit_message>
<xml_diff>
--- a/output_templates/Benefit_Cost_Template.xlsx
+++ b/output_templates/Benefit_Cost_Template.xlsx
@@ -5,30 +5,31 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\soundcast_214\output_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Stefan\Soundcast_feb_twg\output_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19980" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="19980" windowHeight="7530" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Comparison Charts" sheetId="12" r:id="rId1"/>
-    <sheet name="Baseline Metrics" sheetId="1" r:id="rId2"/>
-    <sheet name="Scenario Metrics" sheetId="9" r:id="rId3"/>
-    <sheet name="BaselineScenario" sheetId="13" r:id="rId4"/>
-    <sheet name="Difference" sheetId="10" r:id="rId5"/>
-    <sheet name="HeatResults" sheetId="6" r:id="rId6"/>
-    <sheet name="RawBaseline" sheetId="4" r:id="rId7"/>
-    <sheet name="RawScenario" sheetId="5" r:id="rId8"/>
-    <sheet name="Baseline Charts" sheetId="7" r:id="rId9"/>
-    <sheet name="Scenario Charts" sheetId="11" r:id="rId10"/>
+    <sheet name="Compare Total" sheetId="14" r:id="rId1"/>
+    <sheet name="Comparison Charts" sheetId="12" r:id="rId2"/>
+    <sheet name="Baseline Metrics" sheetId="1" r:id="rId3"/>
+    <sheet name="Scenario Metrics" sheetId="9" r:id="rId4"/>
+    <sheet name="BaselineScenario" sheetId="13" r:id="rId5"/>
+    <sheet name="Difference" sheetId="10" r:id="rId6"/>
+    <sheet name="HeatResults" sheetId="6" r:id="rId7"/>
+    <sheet name="RawBaseline" sheetId="4" r:id="rId8"/>
+    <sheet name="RawScenario" sheetId="5" r:id="rId9"/>
+    <sheet name="Baseline Charts" sheetId="7" r:id="rId10"/>
+    <sheet name="Scenario Charts" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="172">
   <si>
     <t xml:space="preserve">Toll and Auto Operating Cost </t>
   </si>
@@ -621,6 +622,42 @@
   <si>
     <t>Accident Type (per capita)</t>
   </si>
+  <si>
+    <t>Medium Truck Travel Time</t>
+  </si>
+  <si>
+    <t>Medium Truck Operating Cost</t>
+  </si>
+  <si>
+    <t>Medium Truck Tolls</t>
+  </si>
+  <si>
+    <t>Heavy Truck Travel Time</t>
+  </si>
+  <si>
+    <t>Heavy Truck Operating Cost</t>
+  </si>
+  <si>
+    <t>Havey Truck Tolls</t>
+  </si>
+  <si>
+    <t>Baseline Totals</t>
+  </si>
+  <si>
+    <t>Scenario Totals</t>
+  </si>
+  <si>
+    <t>Household Travel Time</t>
+  </si>
+  <si>
+    <t>Household Auto Operating and Tolls</t>
+  </si>
+  <si>
+    <t>Truck Auto Operating and Tolls</t>
+  </si>
+  <si>
+    <t>Truck Travel Time</t>
+  </si>
 </sst>
 </file>
 
@@ -638,7 +675,7 @@
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="169" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1073,7 +1110,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1407,12 +1444,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1422,7 +1453,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7498,10 +7541,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7511,7 +7568,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
@@ -7532,7 +7589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -7569,10 +7626,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T54"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8246,19 +8339,19 @@
       <c r="B20" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="163">
         <f>SUMIF(RawBaseline!$A$23:$A$30,'Baseline Metrics'!$B20,RawBaseline!$D$23:$D$30)</f>
         <v>138281.874327197</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="163">
         <f>SUMIF(RawBaseline!$A$23:$A$30,'Baseline Metrics'!$B20,RawBaseline!$B$23:$B$30)</f>
         <v>20078.151816686699</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="163">
         <f>RawBaseline!B43</f>
         <v>135714</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="163">
         <f>RawBaseline!B63</f>
         <v>19872</v>
       </c>
@@ -8954,7 +9047,7 @@
       <c r="B51" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="84" t="s">
+      <c r="C51" s="45" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="45"/>
@@ -8969,7 +9062,7 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="55" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="C52" s="79"/>
       <c r="D52" s="79"/>
@@ -8980,7 +9073,7 @@
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="55" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C53" s="79"/>
       <c r="D53" s="79"/>
@@ -8990,15 +9083,40 @@
       <c r="H53" s="79"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="119"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79"/>
+      <c r="B54" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="79"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="106"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="79"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="79"/>
+      <c r="F55" s="106"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="106"/>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="118"/>
+      <c r="D57" s="118"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="119"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9007,12 +9125,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10447,17 +10565,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
@@ -10485,7 +10603,7 @@
       <c r="F2" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="157" t="s">
+      <c r="G2" s="155" t="s">
         <v>148</v>
       </c>
       <c r="H2" s="149" t="s">
@@ -10494,7 +10612,7 @@
       <c r="I2" s="149" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="159" t="s">
+      <c r="J2" s="157" t="s">
         <v>158</v>
       </c>
     </row>
@@ -10514,18 +10632,18 @@
         <f>B3-C3</f>
         <v>-6236.314062063524</v>
       </c>
-      <c r="F3" s="157" t="s">
+      <c r="F3" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="160">
+      <c r="G3" s="158">
         <f>B3/'Baseline Metrics'!$C$7*300</f>
         <v>3.1017618744321691</v>
       </c>
-      <c r="H3" s="160">
+      <c r="H3" s="158">
         <f>C3/'Scenario Metrics'!$C$7*300</f>
         <v>2.8268087585748614</v>
       </c>
-      <c r="I3" s="161">
+      <c r="I3" s="159">
         <f>H3-G3</f>
         <v>-0.27495311585730775</v>
       </c>
@@ -10546,18 +10664,18 @@
         <f t="shared" ref="D4:D7" si="0">B4-C4</f>
         <v>-157.78891671233646</v>
       </c>
-      <c r="F4" s="157" t="s">
+      <c r="F4" s="155" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="160">
+      <c r="G4" s="158">
         <f>B4/'Baseline Metrics'!$C$7*300</f>
         <v>8.2132298902646395E-2</v>
       </c>
-      <c r="H4" s="160">
+      <c r="H4" s="158">
         <f>C4/'Scenario Metrics'!$C$7*300</f>
         <v>7.4390016471267431E-2</v>
       </c>
-      <c r="I4" s="161">
+      <c r="I4" s="159">
         <f t="shared" ref="I4:I7" si="1">G4-H4</f>
         <v>7.7422824313789634E-3</v>
       </c>
@@ -10579,18 +10697,18 @@
         <f t="shared" si="0"/>
         <v>-4.8947480773862253</v>
       </c>
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="160">
+      <c r="G5" s="158">
         <f>B5/'Baseline Metrics'!$C$7*300</f>
         <v>2.6509327375729766E-3</v>
       </c>
-      <c r="H5" s="160">
+      <c r="H5" s="158">
         <f>C5/'Scenario Metrics'!$C$7*300</f>
         <v>2.3885845097975991E-3</v>
       </c>
-      <c r="I5" s="161">
+      <c r="I5" s="159">
         <f t="shared" si="1"/>
         <v>2.6234822777537747E-4</v>
       </c>
@@ -10612,18 +10730,18 @@
         <f t="shared" si="0"/>
         <v>-0.1373714621511084</v>
       </c>
-      <c r="F6" s="157" t="s">
+      <c r="F6" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="160">
+      <c r="G6" s="158">
         <f>B6/'Baseline Metrics'!$C$7*300</f>
         <v>8.3432983897194414E-5</v>
       </c>
-      <c r="H6" s="160">
+      <c r="H6" s="158">
         <f>C6/'Scenario Metrics'!$C$7*300</f>
         <v>7.4127285793137708E-5</v>
       </c>
-      <c r="I6" s="161">
+      <c r="I6" s="159">
         <f t="shared" si="1"/>
         <v>9.3056981040567059E-6</v>
       </c>
@@ -10645,18 +10763,18 @@
         <f t="shared" si="0"/>
         <v>-7.2061157104484082</v>
       </c>
-      <c r="F7" s="157" t="s">
+      <c r="F7" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="160">
+      <c r="G7" s="158">
         <f>B7/'Baseline Metrics'!$C$7*300</f>
         <v>3.2950583420717013E-3</v>
       </c>
-      <c r="H7" s="160">
+      <c r="H7" s="158">
         <f>C7/'Scenario Metrics'!$C$7*300</f>
         <v>3.0395099843317994E-3</v>
       </c>
-      <c r="I7" s="161">
+      <c r="I7" s="159">
         <f t="shared" si="1"/>
         <v>2.5554835773990191E-4</v>
       </c>
@@ -10849,25 +10967,25 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A18" s="157" t="s">
+      <c r="A18" s="155" t="s">
         <v>156</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="158" t="s">
+      <c r="C18" s="156" t="s">
         <v>149</v>
       </c>
       <c r="D18" s="149" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="157" t="s">
+      <c r="F18" s="155" t="s">
         <v>159</v>
       </c>
       <c r="G18" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="H18" s="158" t="s">
+      <c r="H18" s="156" t="s">
         <v>149</v>
       </c>
       <c r="I18" s="149" t="s">
@@ -10969,6 +11087,80 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="120" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="121" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="164" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="123" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="165"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="123" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="165"/>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="123" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="165"/>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="123" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="165"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="123" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="165"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="123" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="165"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="123" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="24"/>
+      <c r="C32" s="165"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="165"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="125" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="166"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10976,12 +11168,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11239,7 +11431,7 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="33"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="162">
+      <c r="C10" s="160">
         <f>C4*'Scenario Metrics'!C7</f>
         <v>6766789.5369814029</v>
       </c>
@@ -11283,7 +11475,7 @@
         <f>SUM(E44:E48)</f>
         <v>500957.18922636157</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="40">
         <f>'Scenario Metrics'!N11-'Baseline Metrics'!N11</f>
         <v>-7.4875447193957112E-2</v>
       </c>
@@ -12442,12 +12634,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12567,18 +12759,18 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q12" s="155" t="s">
+      <c r="Q12" s="161" t="s">
         <v>140</v>
       </c>
-      <c r="R12" s="156"/>
-      <c r="S12" s="156"/>
-      <c r="T12" s="156"/>
+      <c r="R12" s="162"/>
+      <c r="S12" s="162"/>
+      <c r="T12" s="162"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q13" s="156"/>
-      <c r="R13" s="156"/>
-      <c r="S13" s="156"/>
-      <c r="T13" s="156"/>
+      <c r="Q13" s="162"/>
+      <c r="R13" s="162"/>
+      <c r="S13" s="162"/>
+      <c r="T13" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12589,7 +12781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L166"/>
   <sheetViews>
@@ -13416,7 +13608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L166"/>
   <sheetViews>
@@ -14240,40 +14432,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>